<commit_message>
Updated the main application methods as well as other requires classes
</commit_message>
<xml_diff>
--- a/Data/ManagerList.xlsx
+++ b/Data/ManagerList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://entuedu-my.sharepoint.com/personal/hu0037ng_e_ntu_edu_sg/Documents/SC4079 - Final Year Project/SC2002/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Modules\Sem 2\SC 2002\SC2002Assignment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_F25DC773A252ABDACC1048D321184AB85ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AED78119-22A7-4087-8472-22F30669F0DB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A1600F-0FDF-4B7C-9C35-C6E527E58126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4057" yWindow="5932" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -384,9 +384,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,7 +408,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -420,7 +425,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>

</xml_diff>